<commit_message>
A basic finished codes for Exp1
</commit_message>
<xml_diff>
--- a/Exp1/data/数据分析.xlsx
+++ b/Exp1/data/数据分析.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ExpMachineLearn\ExpML\Exp1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFC62DB-C8BE-4924-A28F-2D0303A8422E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6216AE83-5B77-4FD9-883B-C53D64B804B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2448" yWindow="288" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据分析" sheetId="1" r:id="rId1"/>
@@ -25,364 +25,369 @@
     <t>industry</t>
   </si>
   <si>
+    <t>initial_list_status</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>唯一性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>有无缺失值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>数值类型/数值分布</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否消去</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>唯一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>预计处理方法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/9000</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_loan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/1526</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>分段or离散</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_of_loan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/2[3, 5]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/1001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>monthly_payment</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/5872</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符/7['B', 'C', 'A', 'G', 'D', 'E', 'F']</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>转换多维向量or离散</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>employer_type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串/6['幼教与中小学校', '政府机构', '上市企业', '普通企业', '世界五百强', '高等教育机构']</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串/14['金融业', '国际组织', '文化和体育业', '建筑业', '电力、热力生产供应业', '批发和零售业', '采矿业', '房地产业', '交通运输、仓储和邮政业', '公共服务、社会组织', '住宿和餐饮业', '信息传输、软件和信息技术服务业', '农、林、牧、渔业', '制造业']</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_year</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串/12[nan, '8 years', '10+ years', '3 years', '7 years', '4 years', '1 year', '&lt; 1 year', '6 years', '2 years', '9 years', '5 years']</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>填充、转换多维向量or离散</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>house_exist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/5[2, 1, 0, 3, 4]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>censor_status</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/3[2, 0, 1]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>issue_date</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期/126(yyyy/mm/dd)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/14[0, 4, 2, 9, 5, 3, 6, 1, 7, 8, 10, 12, 11, 13]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_code</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/786</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>region</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>debt_loan_ratio</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/5822</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>del_in_18month</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/12[0, 3, 1, 4, 2, 9, 5, 6, 7, 8, 10, 15]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>scoring_low</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/132</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>scoring_high</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/360</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>known_outstanding_loan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/47</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>known_dero</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/13[1, 0, 2, 3, 8, 10, 4, 9, 5, 6, 11, 12, 7]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pub_dero_bankrup</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/6[1.0, 0.0, 3.0, 2.0, nan, 5.0]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>填充</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/8558</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>recircle_u</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>实数/2991</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数2[1, 0]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>app_type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/2[0, 1]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>earlies_credit_mon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期/520(mm/dd)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>分段、离散(变成一个时间差值)，约束到月份</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/843</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>policy_code</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仅一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>f0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/3[0.0, nan, 1.0]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/59</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/63</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>early_return</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/6[0, 3, 1, 2, 5, 4]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>early_return_amount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/3967</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>early_return_amount_3mon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数/3484</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDefault(y)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仅从数据来看是否处理</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>loan_id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>recircle_b</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>use</t>
-  </si>
-  <si>
-    <t>recircle_b</t>
-  </si>
-  <si>
-    <t>initial_list_status</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>f1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>f2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>f3</t>
-  </si>
-  <si>
-    <t>f4</t>
-  </si>
-  <si>
-    <t>唯一性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>有无缺失值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>数值类型/数值分布</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否消去</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>唯一</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>预计处理方法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/9000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>total_loan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/1526</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>分段or离散</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_of_loan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/2[3, 5]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/1001</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>monthly_payment</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/5872</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符/7['B', 'C', 'A', 'G', 'D', 'E', 'F']</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>转换多维向量or离散</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>employer_type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串/6['幼教与中小学校', '政府机构', '上市企业', '普通企业', '世界五百强', '高等教育机构']</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串/14['金融业', '国际组织', '文化和体育业', '建筑业', '电力、热力生产供应业', '批发和零售业', '采矿业', '房地产业', '交通运输、仓储和邮政业', '公共服务、社会组织', '住宿和餐饮业', '信息传输、软件和信息技术服务业', '农、林、牧、渔业', '制造业']</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>work_year</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>有</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串/12[nan, '8 years', '10+ years', '3 years', '7 years', '4 years', '1 year', '&lt; 1 year', '6 years', '2 years', '9 years', '5 years']</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>填充、转换多维向量or离散</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>house_exist</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/5[2, 1, 0, 3, 4]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>censor_status</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/3[2, 0, 1]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>issue_date</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期/126(yyyy/mm/dd)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/14[0, 4, 2, 9, 5, 3, 6, 1, 7, 8, 10, 12, 11, 13]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>post_code</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/786</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>region</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>debt_loan_ratio</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/5822</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>del_in_18month</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/12[0, 3, 1, 4, 2, 9, 5, 6, 7, 8, 10, 15]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>scoring_low</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/132</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>scoring_high</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/360</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>known_outstanding_loan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/47</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>known_dero</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/13[1, 0, 2, 3, 8, 10, 4, 9, 5, 6, 11, 12, 7]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pub_dero_bankrup</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/6[1.0, 0.0, 3.0, 2.0, nan, 5.0]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>填充</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/8558</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>recircle_u</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>实数/2991</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数2[1, 0]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>app_type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/2[0, 1]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>earlies_credit_mon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期/520(mm/dd)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>分段、离散(变成一个时间差值)，约束到月份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/843</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>policy_code</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>仅一</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>f0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/3[0.0, nan, 1.0]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/59</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/63</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>early_return</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/6[0, 3, 1, 2, 5, 4]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>early_return_amount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/3967</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>early_return_amount_3mon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数/3484</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>isDefault(y)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>仅从数据来看是否处理</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>loan_id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_id</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -996,7 +1001,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1013,6 +1018,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1372,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1417,199 +1425,199 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1617,650 +1625,650 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
+      <c r="A18" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
         <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
         <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
         <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
         <v>15</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
         <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A basic finished codes for Exp2-1 and Exp2-2
</commit_message>
<xml_diff>
--- a/Exp1/data/数据分析.xlsx
+++ b/Exp1/data/数据分析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ExpMachineLearn\ExpML\Exp1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6216AE83-5B77-4FD9-883B-C53D64B804B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23E81F6-D61C-4B19-A9F5-5E9F97933310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2448" yWindow="288" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6024" yWindow="0" windowWidth="17280" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据分析" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,7 +1007,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,6 +1027,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1381,7 +1390,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1464,7 +1473,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -1750,7 +1759,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B16" t="s">
@@ -1770,7 +1779,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B17" t="s">
@@ -2070,7 +2079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
A basic finished codes for Exp4.
</commit_message>
<xml_diff>
--- a/Exp1/data/数据分析.xlsx
+++ b/Exp1/data/数据分析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ExpMachineLearn\ExpML\Exp1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23E81F6-D61C-4B19-A9F5-5E9F97933310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AED9B3-8B2F-4F81-888F-B3E9BDF81AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6024" yWindow="0" windowWidth="17280" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据分析" sheetId="1" r:id="rId1"/>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>